<commit_message>
Update code for add employee
</commit_message>
<xml_diff>
--- a/Long-NOVEMBER-2020.xlsx
+++ b/Long-NOVEMBER-2020.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t>NAME</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>MON 02/11</t>
+  </si>
+  <si>
+    <t>08:00 - 16:00</t>
   </si>
   <si>
     <t>TUE 03/11</t>
@@ -1294,7 +1297,7 @@
     </row>
     <row r="3">
       <c r="B3" s="95" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
@@ -1312,40 +1315,40 @@
         <v>6</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E4" s="10" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="97"/>
       <c r="C5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>5</v>
-      </c>
       <c r="E5" s="13" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="98"/>
       <c r="C6" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E6" s="16" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="99"/>
       <c r="C7" s="17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>5</v>
@@ -1357,7 +1360,7 @@
     <row r="8">
       <c r="B8" s="100"/>
       <c r="C8" s="20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>5</v>
@@ -1369,7 +1372,7 @@
     <row r="9">
       <c r="B9" s="101"/>
       <c r="C9" s="23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>5</v>
@@ -1381,7 +1384,7 @@
     <row r="10">
       <c r="B10" s="102"/>
       <c r="C10" s="26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>5</v>
@@ -1393,43 +1396,43 @@
     <row r="11">
       <c r="B11" s="103"/>
       <c r="C11" s="29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E11" s="31" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="104"/>
       <c r="C12" s="32" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E12" s="34" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="105"/>
       <c r="C13" s="35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E13" s="37" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="106"/>
       <c r="C14" s="38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D14" s="39" t="s">
         <v>5</v>
@@ -1441,7 +1444,7 @@
     <row r="15">
       <c r="B15" s="107"/>
       <c r="C15" s="41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D15" s="42" t="s">
         <v>5</v>
@@ -1453,7 +1456,7 @@
     <row r="16">
       <c r="B16" s="108"/>
       <c r="C16" s="44" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D16" s="45" t="s">
         <v>5</v>
@@ -1465,7 +1468,7 @@
     <row r="17">
       <c r="B17" s="109"/>
       <c r="C17" s="47" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D17" s="48" t="s">
         <v>5</v>
@@ -1477,43 +1480,43 @@
     <row r="18">
       <c r="B18" s="110"/>
       <c r="C18" s="50" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D18" s="51" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E18" s="52" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="111"/>
       <c r="C19" s="53" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D19" s="54" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E19" s="55" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="112"/>
       <c r="C20" s="56" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D20" s="57" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E20" s="58" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="113"/>
       <c r="C21" s="59" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D21" s="60" t="s">
         <v>5</v>
@@ -1525,7 +1528,7 @@
     <row r="22">
       <c r="B22" s="114"/>
       <c r="C22" s="62" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D22" s="63" t="s">
         <v>5</v>
@@ -1537,7 +1540,7 @@
     <row r="23">
       <c r="B23" s="115"/>
       <c r="C23" s="65" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D23" s="66" t="s">
         <v>5</v>
@@ -1549,7 +1552,7 @@
     <row r="24">
       <c r="B24" s="116"/>
       <c r="C24" s="68" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D24" s="69" t="s">
         <v>5</v>
@@ -1561,43 +1564,43 @@
     <row r="25">
       <c r="B25" s="117"/>
       <c r="C25" s="71" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D25" s="72" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E25" s="73" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="118"/>
       <c r="C26" s="74" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D26" s="75" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E26" s="76" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" s="119"/>
       <c r="C27" s="77" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D27" s="78" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E27" s="79" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="120"/>
       <c r="C28" s="80" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D28" s="81" t="s">
         <v>5</v>
@@ -1609,7 +1612,7 @@
     <row r="29">
       <c r="B29" s="121"/>
       <c r="C29" s="83" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D29" s="84" t="s">
         <v>5</v>
@@ -1621,7 +1624,7 @@
     <row r="30">
       <c r="B30" s="122"/>
       <c r="C30" s="86" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D30" s="87" t="s">
         <v>5</v>
@@ -1633,7 +1636,7 @@
     <row r="31">
       <c r="B31" s="123"/>
       <c r="C31" s="89" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D31" s="90" t="s">
         <v>5</v>
@@ -1645,29 +1648,29 @@
     <row r="32">
       <c r="B32" s="124"/>
       <c r="C32" s="92" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D32" s="93" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E32" s="94" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" s="125" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E33" s="126" t="n">
-        <v>270.0</v>
+        <v>257.0</v>
       </c>
     </row>
     <row r="34">
       <c r="D34" s="127" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E34" s="128" t="n">
-        <v>4860.0</v>
+        <v>4626.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>